<commit_message>
Add firebase dependency and update API endpoints
</commit_message>
<xml_diff>
--- a/public/test.xlsx
+++ b/public/test.xlsx
@@ -1,17 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20325"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DHR-16\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C3FD861C-DFCB-4A81-9069-460B57B5CB79}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>name</t>
   </si>
@@ -44,35 +54,49 @@
   </si>
   <si>
     <t>wetwt</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>akjfa</t>
+  </si>
+  <si>
+    <t>ae</t>
+  </si>
+  <si>
+    <t>oeprja</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
-      <i/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -80,7 +104,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -96,7 +120,13 @@
     </fill>
   </fills>
   <borders count="4">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thick">
         <color rgb="FF000000"/>
@@ -110,6 +140,7 @@
       <bottom style="thick">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -118,9 +149,11 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -135,51 +168,43 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -369,76 +394,129 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="8">
+        <f ca="1">RANDBETWEEN(0,9)</f>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{593B0D1B-D750-4C99-8538-7EF54F915C9E}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="6">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="7">
-        <v>9.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="8">
-        <f>RANDBETWEEN(0,9)</f>
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>